<commit_message>
Added y axis labels
</commit_message>
<xml_diff>
--- a/Nanomole scale synthesis/Nanomole Summary Statistics.xlsx
+++ b/Nanomole scale synthesis/Nanomole Summary Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubai\Documents\Programming\AI3SD\edbo\Nanomole scale synthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303FC046-7417-4B20-A2FB-3714FB5C1787}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92F31C4-2CBA-43AC-B851-841699914BFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,162 +18,64 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$A$12:$D$12</definedName>
-    <definedName name="_xlchart.v1.100" hidden="1">Sheet1!$D$48</definedName>
-    <definedName name="_xlchart.v1.101" hidden="1">Sheet1!$D$49</definedName>
-    <definedName name="_xlchart.v1.102" hidden="1">Sheet1!$D$5</definedName>
-    <definedName name="_xlchart.v1.103" hidden="1">Sheet1!$D$50</definedName>
-    <definedName name="_xlchart.v1.104" hidden="1">Sheet1!$D$51</definedName>
-    <definedName name="_xlchart.v1.105" hidden="1">Sheet1!$D$6</definedName>
-    <definedName name="_xlchart.v1.106" hidden="1">Sheet1!$D$7</definedName>
-    <definedName name="_xlchart.v1.107" hidden="1">Sheet1!$D$8</definedName>
-    <definedName name="_xlchart.v1.108" hidden="1">Sheet1!$D$9</definedName>
-    <definedName name="_xlchart.v1.109" hidden="1">Sheet1!$Q$17</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$A$13:$D$13</definedName>
-    <definedName name="_xlchart.v1.110" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.111" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.112" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.113" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.114" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.115" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.116" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.117" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.118" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.119" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$A$14:$D$14</definedName>
-    <definedName name="_xlchart.v1.120" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.121" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.122" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.123" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.124" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.125" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.126" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.127" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.128" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.129" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$A$15:$D$15</definedName>
-    <definedName name="_xlchart.v1.130" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.131" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.132" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.133" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.134" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.135" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.136" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.137" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.138" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.139" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$A$16:$D$16</definedName>
-    <definedName name="_xlchart.v1.140" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.141" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.142" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.143" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.144" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.145" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.146" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.147" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.148" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.149" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$17:$D$17</definedName>
-    <definedName name="_xlchart.v1.150" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.151" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.152" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.153" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.154" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.155" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.156" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.157" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$A$18:$D$18</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$A$19:$D$19</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$A$20:$D$20</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$A$21:$D$21</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$F$2:$F$51</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$2:$B$51</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$C$2:$C$51</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$D$2:$D$51</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$A$22:$D$22</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$A$23:$D$23</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$A$24:$D$24</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$A$25:$D$25</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$A$26:$D$26</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$A$27:$D$27</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$A$28:$D$28</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$A$29:$D$29</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$A$2:$D$2</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$A$30:$D$30</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$E$2:$E$51</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$F$2:$F$51</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$B$2:$B$51</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$C$2:$C$51</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$A$31:$D$31</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$A$32:$D$32</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$A$33:$D$33</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$A$34:$D$34</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$A$35:$D$35</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$A$36:$D$36</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$A$37:$D$37</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$A$38:$D$38</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$A$39:$D$39</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$A$3:$D$3</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$D$2:$D$51</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$E$2:$E$51</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$F$2:$F$51</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$B$2:$B$51</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$A$40:$D$40</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$A$41:$D$41</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$A$42:$D$42</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$A$43:$D$43</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$A$44:$D$44</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$A$45:$D$45</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$A$46:$D$46</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$A$47:$D$47</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$A$48:$D$48</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$A$49:$D$49</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$C$2:$C$51</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$D$2:$D$51</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$E$2:$E$51</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$F$2:$F$51</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$A$2:$A$51</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$A$4:$D$4</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$A$50:$D$50</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$A$51:$D$51</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$A$5:$D$5</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$A$6:$D$6</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$A$7:$D$7</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$A$8:$D$8</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$A$9:$D$9</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$D$10</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$D$11</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$B$2:$B$51</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$C$2:$C$51</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$D$2:$D$51</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$E$2:$E$51</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$F$2:$F$51</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$D$12</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$D$13</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$D$14</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$D$15</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">Sheet1!$D$16</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">Sheet1!$D$17</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">Sheet1!$D$18</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">Sheet1!$D$19</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">Sheet1!$D$2</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">Sheet1!$D$20</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">Sheet1!$D$21</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">Sheet1!$D$22</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">Sheet1!$D$23</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">Sheet1!$D$24</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">Sheet1!$D$25</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">Sheet1!$D$26</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">Sheet1!$D$27</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">Sheet1!$D$28</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">Sheet1!$D$29</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">Sheet1!$D$2:$D$51</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$10:$D$10</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">Sheet1!$D$3</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">Sheet1!$D$30</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">Sheet1!$D$31</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">Sheet1!$D$32</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">Sheet1!$D$33</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">Sheet1!$D$34</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">Sheet1!$D$35</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">Sheet1!$D$36</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">Sheet1!$D$37</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">Sheet1!$D$38</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$11:$D$11</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">Sheet1!$D$39</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">Sheet1!$D$4</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">Sheet1!$D$40</definedName>
-    <definedName name="_xlchart.v1.93" hidden="1">Sheet1!$D$41</definedName>
-    <definedName name="_xlchart.v1.94" hidden="1">Sheet1!$D$42</definedName>
-    <definedName name="_xlchart.v1.95" hidden="1">Sheet1!$D$43</definedName>
-    <definedName name="_xlchart.v1.96" hidden="1">Sheet1!$D$44</definedName>
-    <definedName name="_xlchart.v1.97" hidden="1">Sheet1!$D$45</definedName>
-    <definedName name="_xlchart.v1.98" hidden="1">Sheet1!$D$46</definedName>
-    <definedName name="_xlchart.v1.99" hidden="1">Sheet1!$D$47</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$E$2:$E$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -194,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Random</t>
   </si>
@@ -206,6 +108,12 @@
   </si>
   <si>
     <t>EI (0 default)</t>
+  </si>
+  <si>
+    <t>TS (0 default)</t>
+  </si>
+  <si>
+    <t>TS</t>
   </si>
 </sst>
 </file>
@@ -251,9 +159,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFB8FC0"/>
+      <color rgb="FFF72585"/>
+      <color rgb="FFB95FF7"/>
+      <color rgb="FF7209B7"/>
+      <color rgb="FF98A8F6"/>
+      <color rgb="FF4361EE"/>
       <color rgb="FFFA7EB6"/>
-      <color rgb="FF7209B7"/>
-      <color rgb="FFF72585"/>
       <color rgb="FFC983F9"/>
       <color rgb="FFA939F5"/>
       <color rgb="FF4CC9F0"/>
@@ -275,38 +187,48 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.151</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.153</cx:f>
+        <cx:f>_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.155</cx:f>
+        <cx:f>_xlchart.v1.29</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.157</cx:f>
+        <cx:f>_xlchart.v1.31</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="4">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.33</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="5">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{F2EF0EF9-513A-4382-B4D4-E2B15A9ED507}">
+        <cx:series layoutId="boxWhisker" uniqueId="{22423F98-09F0-4F7B-B383-DFDFBEFE47F8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.150</cx:f>
+              <cx:f>_xlchart.v1.24</cx:f>
               <cx:v>Random (0 default)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
             <a:solidFill>
-              <a:srgbClr val="FA7EB6"/>
+              <a:srgbClr val="FB8FC0"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -320,16 +242,16 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{20A0119D-0181-4364-908B-462C409850E3}">
+        <cx:series layoutId="boxWhisker" uniqueId="{9A7A3C81-ECB1-49E9-8FE0-FD0E14581AC0}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.152</cx:f>
+              <cx:f>_xlchart.v1.26</cx:f>
               <cx:v>EI (0 default)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:spPr>
             <a:solidFill>
-              <a:srgbClr val="C983F9"/>
+              <a:srgbClr val="B95FF7"/>
             </a:solidFill>
             <a:ln>
               <a:solidFill>
@@ -343,10 +265,33 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{2892B2C8-A00B-47CA-B264-E2690E0D8673}">
+        <cx:series layoutId="boxWhisker" uniqueId="{0D5505C0-5F3B-457A-A003-F9D8F4DB9CDB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.154</cx:f>
+              <cx:f>_xlchart.v1.28</cx:f>
+              <cx:v>TS (0 default)</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:srgbClr val="98A8F6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{C8EDC47F-602A-4C31-B01A-0B34A7883258}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.30</cx:f>
               <cx:v>Random</cx:v>
             </cx:txData>
           </cx:tx>
@@ -360,16 +305,16 @@
               </a:solidFill>
             </a:ln>
           </cx:spPr>
-          <cx:dataId val="2"/>
+          <cx:dataId val="3"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{6F667C92-4E1D-42A8-8A72-037B862F5602}">
+        <cx:series layoutId="boxWhisker" uniqueId="{E67AFBD2-EBC2-416F-8E7A-4686CAD8B1C0}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.156</cx:f>
+              <cx:f>_xlchart.v1.32</cx:f>
               <cx:v>EI</cx:v>
             </cx:txData>
           </cx:tx>
@@ -383,7 +328,30 @@
               </a:solidFill>
             </a:ln>
           </cx:spPr>
-          <cx:dataId val="3"/>
+          <cx:dataId val="4"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{FDB306FC-AFA9-4792-9CC5-292329440FE9}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.34</cx:f>
+              <cx:v>TS</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4361EE"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="5"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
@@ -391,11 +359,39 @@
         </cx:series>
       </cx:plotAreaRegion>
       <cx:axis id="0" hidden="1">
-        <cx:catScaling gapWidth="1"/>
+        <cx:catScaling gapWidth="0.0500000007"/>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>MISER Area Count</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1200"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>MISER Area Count</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
@@ -964,25 +960,25 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="5" name="Chart 4">
+            <xdr:cNvPr id="2" name="Chart 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41BCB43E-D12D-45DB-A6EC-C0CDD8B700C6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EE9BB23-442B-4381-944A-2C6E74C20FBB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1009,8 +1005,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3444240" y="7311390"/>
-              <a:ext cx="3329940" cy="2743200"/>
+              <a:off x="4351020" y="6297930"/>
+              <a:ext cx="4572000" cy="3859530"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1306,15 +1302,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1322,13 +1318,19 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3295</v>
       </c>
@@ -1336,13 +1338,19 @@
         <v>9651</v>
       </c>
       <c r="C2">
+        <v>4299</v>
+      </c>
+      <c r="D2">
         <v>1331</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2847</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>10238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>19040</v>
       </c>
@@ -1350,13 +1358,19 @@
         <v>8663</v>
       </c>
       <c r="C3">
+        <v>9651</v>
+      </c>
+      <c r="D3">
         <v>4811</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>5607</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4573</v>
       </c>
@@ -1364,13 +1378,19 @@
         <v>6096</v>
       </c>
       <c r="C4">
+        <v>19040</v>
+      </c>
+      <c r="D4">
         <v>9651</v>
       </c>
-      <c r="D4">
-        <v>10238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>10238</v>
+      </c>
+      <c r="F4">
+        <v>4811</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3301</v>
       </c>
@@ -1378,13 +1398,19 @@
         <v>9651</v>
       </c>
       <c r="C5">
+        <v>6096</v>
+      </c>
+      <c r="D5">
         <v>3288</v>
       </c>
-      <c r="D5">
-        <v>10238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>10238</v>
+      </c>
+      <c r="F5">
+        <v>19040</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1308</v>
       </c>
@@ -1392,13 +1418,19 @@
         <v>1156</v>
       </c>
       <c r="C6">
+        <v>1121</v>
+      </c>
+      <c r="D6">
         <v>2390</v>
       </c>
-      <c r="D6">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>14394</v>
+      </c>
+      <c r="F6">
+        <v>10238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4276</v>
       </c>
@@ -1406,13 +1438,19 @@
         <v>19040</v>
       </c>
       <c r="C7">
+        <v>1121</v>
+      </c>
+      <c r="D7">
         <v>5837</v>
       </c>
-      <c r="D7">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>14394</v>
+      </c>
+      <c r="F7">
+        <v>10238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>753</v>
       </c>
@@ -1420,13 +1458,19 @@
         <v>6096</v>
       </c>
       <c r="C8">
+        <v>19040</v>
+      </c>
+      <c r="D8">
         <v>6509</v>
       </c>
-      <c r="D8">
-        <v>10238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>10238</v>
+      </c>
+      <c r="F8">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4883</v>
       </c>
@@ -1434,13 +1478,19 @@
         <v>6509</v>
       </c>
       <c r="C9">
+        <v>9651</v>
+      </c>
+      <c r="D9">
         <v>7781</v>
       </c>
-      <c r="D9">
-        <v>10238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>10238</v>
+      </c>
+      <c r="F9">
+        <v>10238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>978</v>
       </c>
@@ -1448,13 +1498,19 @@
         <v>14394</v>
       </c>
       <c r="C10">
+        <v>9651</v>
+      </c>
+      <c r="D10">
         <v>4225</v>
       </c>
-      <c r="D10">
-        <v>19040</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>19040</v>
+      </c>
+      <c r="F10">
+        <v>19040</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1794</v>
       </c>
@@ -1462,13 +1518,19 @@
         <v>10238</v>
       </c>
       <c r="C11">
+        <v>10238</v>
+      </c>
+      <c r="D11">
         <v>3301</v>
       </c>
-      <c r="D11">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>14394</v>
+      </c>
+      <c r="F11">
+        <v>6096</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3059</v>
       </c>
@@ -1476,13 +1538,19 @@
         <v>14394</v>
       </c>
       <c r="C12">
+        <v>10238</v>
+      </c>
+      <c r="D12">
         <v>5050</v>
       </c>
-      <c r="D12">
-        <v>6096</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>6096</v>
+      </c>
+      <c r="F12">
+        <v>19040</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5716</v>
       </c>
@@ -1490,13 +1558,19 @@
         <v>14394</v>
       </c>
       <c r="C13">
+        <v>10238</v>
+      </c>
+      <c r="D13">
         <v>7781</v>
       </c>
-      <c r="D13">
-        <v>10238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>10238</v>
+      </c>
+      <c r="F13">
+        <v>10238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14394</v>
       </c>
@@ -1504,13 +1578,19 @@
         <v>14394</v>
       </c>
       <c r="C14">
+        <v>14394</v>
+      </c>
+      <c r="D14">
         <v>4883</v>
       </c>
-      <c r="D14">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>14394</v>
+      </c>
+      <c r="F14">
+        <v>6096</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1428</v>
       </c>
@@ -1518,13 +1598,19 @@
         <v>1026</v>
       </c>
       <c r="C15">
+        <v>4811</v>
+      </c>
+      <c r="D15">
         <v>6737</v>
       </c>
-      <c r="D15">
-        <v>6096</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>6096</v>
+      </c>
+      <c r="F15">
+        <v>4882</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4573</v>
       </c>
@@ -1532,13 +1618,19 @@
         <v>726</v>
       </c>
       <c r="C16">
+        <v>857</v>
+      </c>
+      <c r="D16">
         <v>4935</v>
       </c>
-      <c r="D16">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>14394</v>
+      </c>
+      <c r="F16">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4811</v>
       </c>
@@ -1546,13 +1638,19 @@
         <v>1156</v>
       </c>
       <c r="C17">
+        <v>1541</v>
+      </c>
+      <c r="D17">
         <v>4396</v>
       </c>
-      <c r="D17">
-        <v>6096</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>6096</v>
+      </c>
+      <c r="F17">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>730</v>
       </c>
@@ -1560,13 +1658,19 @@
         <v>14394</v>
       </c>
       <c r="C18">
+        <v>9651</v>
+      </c>
+      <c r="D18">
         <v>4206</v>
       </c>
-      <c r="D18">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>14394</v>
+      </c>
+      <c r="F18">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1039</v>
       </c>
@@ -1574,13 +1678,19 @@
         <v>857</v>
       </c>
       <c r="C19">
+        <v>6096</v>
+      </c>
+      <c r="D19">
         <v>6459</v>
       </c>
-      <c r="D19">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>14394</v>
+      </c>
+      <c r="F19">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1026</v>
       </c>
@@ -1588,13 +1698,19 @@
         <v>4396</v>
       </c>
       <c r="C20">
+        <v>6096</v>
+      </c>
+      <c r="D20">
         <v>2204</v>
       </c>
-      <c r="D20">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>14394</v>
+      </c>
+      <c r="F20">
+        <v>4882</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7781</v>
       </c>
@@ -1602,13 +1718,19 @@
         <v>14394</v>
       </c>
       <c r="C21">
+        <v>14394</v>
+      </c>
+      <c r="D21">
         <v>4680</v>
       </c>
-      <c r="D21">
-        <v>6096</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>6096</v>
+      </c>
+      <c r="F21">
+        <v>10238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2492</v>
       </c>
@@ -1616,13 +1738,19 @@
         <v>726</v>
       </c>
       <c r="C22">
+        <v>4396</v>
+      </c>
+      <c r="D22">
         <v>8663</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>677</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>9651</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>840</v>
       </c>
@@ -1630,13 +1758,19 @@
         <v>14394</v>
       </c>
       <c r="C23">
+        <v>1485</v>
+      </c>
+      <c r="D23">
         <v>6459</v>
       </c>
-      <c r="D23">
-        <v>6096</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>6096</v>
+      </c>
+      <c r="F23">
+        <v>9651</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2699</v>
       </c>
@@ -1644,13 +1778,19 @@
         <v>1121</v>
       </c>
       <c r="C24">
-        <v>6096</v>
+        <v>14394</v>
       </c>
       <c r="D24">
+        <v>6096</v>
+      </c>
+      <c r="E24">
         <v>1121</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>496</v>
       </c>
@@ -1658,13 +1798,19 @@
         <v>14394</v>
       </c>
       <c r="C25">
+        <v>2052</v>
+      </c>
+      <c r="D25">
         <v>2390</v>
       </c>
-      <c r="D25">
-        <v>19040</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>19040</v>
+      </c>
+      <c r="F25">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1521</v>
       </c>
@@ -1672,13 +1818,19 @@
         <v>6096</v>
       </c>
       <c r="C26">
+        <v>4396</v>
+      </c>
+      <c r="D26">
         <v>4413</v>
       </c>
-      <c r="D26">
-        <v>6096</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>6096</v>
+      </c>
+      <c r="F26">
+        <v>6096</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8663</v>
       </c>
@@ -1686,13 +1838,19 @@
         <v>14394</v>
       </c>
       <c r="C27">
+        <v>14394</v>
+      </c>
+      <c r="D27">
         <v>4396</v>
       </c>
-      <c r="D27">
-        <v>19040</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>19040</v>
+      </c>
+      <c r="F27">
+        <v>8706</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>7781</v>
       </c>
@@ -1700,13 +1858,19 @@
         <v>14394</v>
       </c>
       <c r="C28">
-        <v>6096</v>
+        <v>2002</v>
       </c>
       <c r="D28">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6096</v>
+      </c>
+      <c r="E28">
+        <v>14394</v>
+      </c>
+      <c r="F28">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5607</v>
       </c>
@@ -1714,13 +1878,19 @@
         <v>857</v>
       </c>
       <c r="C29">
+        <v>2847</v>
+      </c>
+      <c r="D29">
         <v>8706</v>
       </c>
-      <c r="D29">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>14394</v>
+      </c>
+      <c r="F29">
+        <v>19040</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10238</v>
       </c>
@@ -1728,13 +1898,19 @@
         <v>10238</v>
       </c>
       <c r="C30">
+        <v>10238</v>
+      </c>
+      <c r="D30">
         <v>2054</v>
       </c>
-      <c r="D30">
-        <v>19040</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>19040</v>
+      </c>
+      <c r="F30">
+        <v>19040</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8354</v>
       </c>
@@ -1742,13 +1918,19 @@
         <v>9651</v>
       </c>
       <c r="C31">
+        <v>8663</v>
+      </c>
+      <c r="D31">
         <v>2699</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>9651</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <v>4396</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>8663</v>
       </c>
@@ -1756,13 +1938,19 @@
         <v>1428</v>
       </c>
       <c r="C32">
+        <v>2847</v>
+      </c>
+      <c r="D32">
         <v>5837</v>
       </c>
-      <c r="D32">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>14394</v>
+      </c>
+      <c r="F32">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5479</v>
       </c>
@@ -1770,13 +1958,19 @@
         <v>14394</v>
       </c>
       <c r="C33">
-        <v>6096</v>
+        <v>14394</v>
       </c>
       <c r="D33">
-        <v>19040</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6096</v>
+      </c>
+      <c r="E33">
+        <v>19040</v>
+      </c>
+      <c r="F33">
+        <v>4083</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2415</v>
       </c>
@@ -1784,13 +1978,19 @@
         <v>19040</v>
       </c>
       <c r="C34">
+        <v>9651</v>
+      </c>
+      <c r="D34">
         <v>2178</v>
       </c>
-      <c r="D34">
-        <v>19040</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>19040</v>
+      </c>
+      <c r="F34">
+        <v>6096</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4413</v>
       </c>
@@ -1798,13 +1998,19 @@
         <v>4882</v>
       </c>
       <c r="C35">
+        <v>19040</v>
+      </c>
+      <c r="D35">
         <v>4206</v>
       </c>
-      <c r="D35">
-        <v>6096</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>6096</v>
+      </c>
+      <c r="F35">
+        <v>19040</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1136</v>
       </c>
@@ -1812,13 +2018,19 @@
         <v>924</v>
       </c>
       <c r="C36">
+        <v>19040</v>
+      </c>
+      <c r="D36">
         <v>5479</v>
       </c>
-      <c r="D36">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>14394</v>
+      </c>
+      <c r="F36">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>5704</v>
       </c>
@@ -1826,13 +2038,19 @@
         <v>10238</v>
       </c>
       <c r="C37">
+        <v>10238</v>
+      </c>
+      <c r="D37">
         <v>6478</v>
       </c>
-      <c r="D37">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>14394</v>
+      </c>
+      <c r="F37">
+        <v>6478</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1414</v>
       </c>
@@ -1840,13 +2058,19 @@
         <v>4168</v>
       </c>
       <c r="C38">
+        <v>2431</v>
+      </c>
+      <c r="D38">
         <v>4168</v>
       </c>
-      <c r="D38">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>14394</v>
+      </c>
+      <c r="F38">
+        <v>9651</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1449</v>
       </c>
@@ -1854,13 +2078,19 @@
         <v>2996</v>
       </c>
       <c r="C39">
-        <v>7781</v>
+        <v>2847</v>
       </c>
       <c r="D39">
         <v>7781</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>7781</v>
+      </c>
+      <c r="F39">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>3059</v>
       </c>
@@ -1868,13 +2098,19 @@
         <v>10238</v>
       </c>
       <c r="C40">
+        <v>10238</v>
+      </c>
+      <c r="D40">
         <v>6478</v>
       </c>
-      <c r="D40">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>14394</v>
+      </c>
+      <c r="F40">
+        <v>19040</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1638</v>
       </c>
@@ -1882,13 +2118,19 @@
         <v>14394</v>
       </c>
       <c r="C41">
+        <v>14394</v>
+      </c>
+      <c r="D41">
         <v>4680</v>
       </c>
-      <c r="D41">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>14394</v>
+      </c>
+      <c r="F41">
+        <v>19040</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>5837</v>
       </c>
@@ -1896,13 +2138,19 @@
         <v>2204</v>
       </c>
       <c r="C42">
+        <v>14394</v>
+      </c>
+      <c r="D42">
         <v>4225</v>
       </c>
-      <c r="D42">
-        <v>19040</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>19040</v>
+      </c>
+      <c r="F42">
+        <v>19040</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4396</v>
       </c>
@@ -1910,13 +2158,19 @@
         <v>6096</v>
       </c>
       <c r="C43">
+        <v>6096</v>
+      </c>
+      <c r="D43">
         <v>5837</v>
       </c>
-      <c r="D43">
-        <v>19040</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>19040</v>
+      </c>
+      <c r="F43">
+        <v>19040</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>6509</v>
       </c>
@@ -1924,13 +2178,19 @@
         <v>2847</v>
       </c>
       <c r="C44">
+        <v>14394</v>
+      </c>
+      <c r="D44">
         <v>6084</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>7781</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F44">
+        <v>10238</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>5704</v>
       </c>
@@ -1938,13 +2198,19 @@
         <v>14394</v>
       </c>
       <c r="C45">
+        <v>2847</v>
+      </c>
+      <c r="D45">
         <v>7781</v>
       </c>
-      <c r="D45">
-        <v>10238</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>10238</v>
+      </c>
+      <c r="F45">
+        <v>6096</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>8663</v>
       </c>
@@ -1952,13 +2218,19 @@
         <v>857</v>
       </c>
       <c r="C46">
+        <v>2002</v>
+      </c>
+      <c r="D46">
         <v>2847</v>
       </c>
-      <c r="D46">
-        <v>10238</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>10238</v>
+      </c>
+      <c r="F46">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>796</v>
       </c>
@@ -1966,13 +2238,19 @@
         <v>19040</v>
       </c>
       <c r="C47">
+        <v>14394</v>
+      </c>
+      <c r="D47">
         <v>5716</v>
       </c>
-      <c r="D47">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>14394</v>
+      </c>
+      <c r="F47">
+        <v>4168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1899</v>
       </c>
@@ -1980,13 +2258,19 @@
         <v>14394</v>
       </c>
       <c r="C48">
+        <v>14394</v>
+      </c>
+      <c r="D48">
         <v>4680</v>
       </c>
-      <c r="D48">
-        <v>6096</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>6096</v>
+      </c>
+      <c r="F48">
+        <v>14394</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4168</v>
       </c>
@@ -1994,13 +2278,19 @@
         <v>14394</v>
       </c>
       <c r="C49">
+        <v>6096</v>
+      </c>
+      <c r="D49">
         <v>6028</v>
       </c>
-      <c r="D49">
-        <v>6096</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>6096</v>
+      </c>
+      <c r="F49">
+        <v>6096</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>825</v>
       </c>
@@ -2008,13 +2298,19 @@
         <v>6096</v>
       </c>
       <c r="C50">
+        <v>4396</v>
+      </c>
+      <c r="D50">
         <v>6509</v>
       </c>
-      <c r="D50">
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>14394</v>
+      </c>
+      <c r="F50">
+        <v>10238</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4413</v>
       </c>
@@ -2022,22 +2318,16 @@
         <v>6096</v>
       </c>
       <c r="C51">
+        <v>10238</v>
+      </c>
+      <c r="D51">
         <v>7781</v>
       </c>
-      <c r="D51">
-        <v>19040</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D53">
-        <f>MEDIAN(D2:D51)</f>
-        <v>14394</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D54">
-        <f>_xlfn.QUARTILE.EXC(D2:D51,1)</f>
-        <v>6096</v>
+      <c r="E51">
+        <v>19040</v>
+      </c>
+      <c r="F51">
+        <v>6028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>